<commit_message>
change GTIN cell format from number to text
</commit_message>
<xml_diff>
--- a/normalized-data/square-mass-import-catalog_usa.xlsx
+++ b/normalized-data/square-mass-import-catalog_usa.xlsx
@@ -1484,9 +1484,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1541,6 +1542,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1591,7 +1593,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1624,8 +1626,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1711,28 +1717,28 @@
   </sheetPr>
   <dimension ref="A2:AF107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L105" activeCellId="0" sqref="L105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="36.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="186.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="101.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="51.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="186.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="62.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="37.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="94.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="38.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="51.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="186.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="36.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="22.43"/>
@@ -2043,7 +2049,7 @@
       <c r="J7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="9" t="n">
         <v>14109604604858</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -2111,7 +2117,7 @@
       <c r="J8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="9" t="n">
         <v>14202221654343</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -2167,7 +2173,7 @@
       <c r="J9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="9" t="n">
         <v>10289338790688</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -2223,7 +2229,7 @@
       <c r="J10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="9" t="n">
         <v>40290832470549</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -2279,7 +2285,7 @@
       <c r="J11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="9" t="n">
         <v>84207900225560</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -2335,7 +2341,7 @@
       <c r="J12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="9" t="n">
         <v>14722003109376</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -2391,7 +2397,7 @@
       <c r="J13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="9" t="n">
         <v>73777516987868</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -2447,7 +2453,7 @@
       <c r="J14" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="9" t="n">
         <v>51162143363027</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -2503,7 +2509,7 @@
       <c r="J15" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="9" t="n">
         <v>99305262963586</v>
       </c>
       <c r="L15" s="2" t="s">
@@ -2559,7 +2565,7 @@
       <c r="J16" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="9" t="n">
         <v>42132902332521</v>
       </c>
       <c r="L16" s="2" t="s">
@@ -2615,7 +2621,7 @@
       <c r="J17" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="9" t="n">
         <v>49257718277257</v>
       </c>
       <c r="L17" s="2" t="s">
@@ -2671,7 +2677,7 @@
       <c r="J18" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="9" t="n">
         <v>23580959145415</v>
       </c>
       <c r="L18" s="2" t="s">
@@ -2727,7 +2733,7 @@
       <c r="J19" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="9" t="n">
         <v>69125978120871</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -2783,7 +2789,7 @@
       <c r="J20" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="9" t="n">
         <v>65859647272720</v>
       </c>
       <c r="L20" s="2" t="s">
@@ -2839,7 +2845,7 @@
       <c r="J21" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="9" t="n">
         <v>80157313608196</v>
       </c>
       <c r="L21" s="2" t="s">
@@ -2895,7 +2901,7 @@
       <c r="J22" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="9" t="n">
         <v>58468893137835</v>
       </c>
       <c r="L22" s="2" t="s">
@@ -2951,7 +2957,7 @@
       <c r="J23" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="9" t="n">
         <v>24655840280891</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -3007,7 +3013,7 @@
       <c r="J24" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="9" t="n">
         <v>93490705034401</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -3063,7 +3069,7 @@
       <c r="J25" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="9" t="n">
         <v>73105115630711</v>
       </c>
       <c r="L25" s="2" t="s">
@@ -3119,7 +3125,7 @@
       <c r="J26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="9" t="n">
         <v>86685277622874</v>
       </c>
       <c r="L26" s="2" t="s">
@@ -3175,7 +3181,7 @@
       <c r="J27" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="9" t="n">
         <v>23761784959629</v>
       </c>
       <c r="L27" s="2" t="s">
@@ -3231,7 +3237,7 @@
       <c r="J28" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="K28" s="9" t="n">
         <v>51080830461219</v>
       </c>
       <c r="L28" s="2" t="s">
@@ -3287,7 +3293,7 @@
       <c r="J29" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="K29" s="9" t="n">
         <v>41418400223058</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -3343,7 +3349,7 @@
       <c r="J30" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K30" s="9" t="n">
         <v>93758042485807</v>
       </c>
       <c r="L30" s="2" t="s">
@@ -3399,7 +3405,7 @@
       <c r="J31" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="K31" s="9" t="n">
         <v>52171972512477</v>
       </c>
       <c r="L31" s="2" t="s">
@@ -3455,7 +3461,7 @@
       <c r="J32" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K32" s="9" t="n">
         <v>21583519874323</v>
       </c>
       <c r="L32" s="2" t="s">
@@ -3511,7 +3517,7 @@
       <c r="J33" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="K33" s="9" t="n">
         <v>26736626793030</v>
       </c>
       <c r="L33" s="2" t="s">
@@ -3567,7 +3573,7 @@
       <c r="J34" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K34" s="9" t="n">
         <v>12284011325362</v>
       </c>
       <c r="L34" s="2" t="s">
@@ -3623,7 +3629,7 @@
       <c r="J35" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="K35" s="9" t="n">
         <v>53666117476789</v>
       </c>
       <c r="L35" s="2" t="s">
@@ -3679,7 +3685,7 @@
       <c r="J36" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="K36" s="9" t="n">
         <v>75970202836561</v>
       </c>
       <c r="L36" s="2" t="s">
@@ -3735,7 +3741,7 @@
       <c r="J37" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="K37" s="9" t="n">
         <v>61327144407778</v>
       </c>
       <c r="L37" s="2" t="s">
@@ -3791,7 +3797,7 @@
       <c r="J38" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="K38" s="9" t="n">
         <v>45788508647136</v>
       </c>
       <c r="L38" s="2" t="s">
@@ -3847,7 +3853,7 @@
       <c r="J39" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="K39" s="9" t="n">
         <v>20127249361160</v>
       </c>
       <c r="L39" s="2" t="s">
@@ -3903,7 +3909,7 @@
       <c r="J40" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="K40" s="9" t="n">
         <v>62190360827574</v>
       </c>
       <c r="L40" s="2" t="s">
@@ -3959,7 +3965,7 @@
       <c r="J41" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="K41" s="9" t="n">
         <v>19459747163476</v>
       </c>
       <c r="L41" s="2" t="s">
@@ -4015,7 +4021,7 @@
       <c r="J42" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="K42" s="0" t="n">
+      <c r="K42" s="9" t="n">
         <v>46746380394391</v>
       </c>
       <c r="L42" s="2" t="s">
@@ -4071,7 +4077,7 @@
       <c r="J43" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="K43" s="0" t="n">
+      <c r="K43" s="9" t="n">
         <v>20256258825006</v>
       </c>
       <c r="L43" s="2" t="s">
@@ -4127,7 +4133,7 @@
       <c r="J44" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="K44" s="0" t="n">
+      <c r="K44" s="9" t="n">
         <v>71473469057315</v>
       </c>
       <c r="L44" s="2" t="s">
@@ -4183,7 +4189,7 @@
       <c r="J45" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K45" s="0" t="n">
+      <c r="K45" s="9" t="n">
         <v>35224346795683</v>
       </c>
       <c r="L45" s="2" t="s">
@@ -4239,7 +4245,7 @@
       <c r="J46" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="K46" s="0" t="n">
+      <c r="K46" s="9" t="n">
         <v>45734082687422</v>
       </c>
       <c r="L46" s="2" t="s">
@@ -4295,7 +4301,7 @@
       <c r="J47" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K47" s="0" t="n">
+      <c r="K47" s="9" t="n">
         <v>25090603661905</v>
       </c>
       <c r="L47" s="2" t="s">
@@ -4351,7 +4357,7 @@
       <c r="J48" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="K48" s="0" t="n">
+      <c r="K48" s="9" t="n">
         <v>84952970015668</v>
       </c>
       <c r="L48" s="2" t="s">
@@ -4407,7 +4413,7 @@
       <c r="J49" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K49" s="0" t="n">
+      <c r="K49" s="9" t="n">
         <v>76416879474381</v>
       </c>
       <c r="L49" s="2" t="s">
@@ -4463,7 +4469,7 @@
       <c r="J50" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="K50" s="9" t="n">
         <v>16269018549201</v>
       </c>
       <c r="L50" s="2" t="s">
@@ -4519,7 +4525,7 @@
       <c r="J51" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="K51" s="0" t="n">
+      <c r="K51" s="9" t="n">
         <v>36007938913287</v>
       </c>
       <c r="L51" s="2" t="s">
@@ -4575,7 +4581,7 @@
       <c r="J52" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="K52" s="0" t="n">
+      <c r="K52" s="9" t="n">
         <v>24525747669281</v>
       </c>
       <c r="L52" s="2" t="s">
@@ -4631,7 +4637,7 @@
       <c r="J53" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="K53" s="0" t="n">
+      <c r="K53" s="9" t="n">
         <v>26196313329786</v>
       </c>
       <c r="L53" s="2" t="s">
@@ -4687,7 +4693,7 @@
       <c r="J54" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="K54" s="0" t="n">
+      <c r="K54" s="9" t="n">
         <v>20862838477345</v>
       </c>
       <c r="L54" s="2" t="s">
@@ -4743,7 +4749,7 @@
       <c r="J55" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="K55" s="0" t="n">
+      <c r="K55" s="9" t="n">
         <v>36037284563664</v>
       </c>
       <c r="L55" s="2" t="s">
@@ -4799,7 +4805,7 @@
       <c r="J56" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="K56" s="0" t="n">
+      <c r="K56" s="9" t="n">
         <v>13193681859339</v>
       </c>
       <c r="L56" s="2" t="s">
@@ -4855,7 +4861,7 @@
       <c r="J57" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="K57" s="0" t="n">
+      <c r="K57" s="9" t="n">
         <v>86763178062714</v>
       </c>
       <c r="L57" s="2" t="s">
@@ -4911,7 +4917,7 @@
       <c r="J58" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="K58" s="0" t="n">
+      <c r="K58" s="9" t="n">
         <v>20530814931315</v>
       </c>
       <c r="L58" s="2" t="s">
@@ -4967,7 +4973,7 @@
       <c r="J59" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="K59" s="0" t="n">
+      <c r="K59" s="9" t="n">
         <v>63318658338474</v>
       </c>
       <c r="L59" s="2" t="s">
@@ -5023,7 +5029,7 @@
       <c r="J60" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="K60" s="0" t="n">
+      <c r="K60" s="9" t="n">
         <v>16310871290403</v>
       </c>
       <c r="L60" s="2" t="s">
@@ -5079,7 +5085,7 @@
       <c r="J61" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="K61" s="0" t="n">
+      <c r="K61" s="9" t="n">
         <v>65940494145215</v>
       </c>
       <c r="L61" s="2" t="s">
@@ -5135,7 +5141,7 @@
       <c r="J62" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="K62" s="0" t="n">
+      <c r="K62" s="9" t="n">
         <v>22515530946973</v>
       </c>
       <c r="L62" s="2" t="s">
@@ -5191,7 +5197,7 @@
       <c r="J63" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="K63" s="0" t="n">
+      <c r="K63" s="9" t="n">
         <v>76547149292154</v>
       </c>
       <c r="L63" s="2" t="s">
@@ -5247,7 +5253,7 @@
       <c r="J64" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="K64" s="0" t="n">
+      <c r="K64" s="9" t="n">
         <v>92842924373813</v>
       </c>
       <c r="L64" s="2" t="s">
@@ -5303,7 +5309,7 @@
       <c r="J65" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="K65" s="0" t="n">
+      <c r="K65" s="9" t="n">
         <v>73064086186736</v>
       </c>
       <c r="L65" s="2" t="s">
@@ -5359,7 +5365,7 @@
       <c r="J66" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="K66" s="0" t="n">
+      <c r="K66" s="9" t="n">
         <v>13567700390896</v>
       </c>
       <c r="L66" s="2" t="s">
@@ -5415,7 +5421,7 @@
       <c r="J67" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="K67" s="0" t="n">
+      <c r="K67" s="9" t="n">
         <v>52280020167217</v>
       </c>
       <c r="L67" s="2" t="s">
@@ -5471,7 +5477,7 @@
       <c r="J68" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K68" s="0" t="n">
+      <c r="K68" s="9" t="n">
         <v>55225619530351</v>
       </c>
       <c r="L68" s="2" t="s">
@@ -5527,7 +5533,7 @@
       <c r="J69" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="K69" s="0" t="n">
+      <c r="K69" s="9" t="n">
         <v>66882207361884</v>
       </c>
       <c r="L69" s="2" t="s">
@@ -5583,7 +5589,7 @@
       <c r="J70" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="K70" s="0" t="n">
+      <c r="K70" s="9" t="n">
         <v>19263536217596</v>
       </c>
       <c r="L70" s="2" t="s">
@@ -5639,7 +5645,7 @@
       <c r="J71" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="K71" s="0" t="n">
+      <c r="K71" s="9" t="n">
         <v>88129625450959</v>
       </c>
       <c r="L71" s="2" t="s">
@@ -5695,7 +5701,7 @@
       <c r="J72" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="K72" s="0" t="n">
+      <c r="K72" s="9" t="n">
         <v>67801006981945</v>
       </c>
       <c r="L72" s="2" t="s">
@@ -5751,7 +5757,7 @@
       <c r="J73" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="K73" s="0" t="n">
+      <c r="K73" s="9" t="n">
         <v>62159138423123</v>
       </c>
       <c r="L73" s="2" t="s">
@@ -5807,7 +5813,7 @@
       <c r="J74" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="K74" s="0" t="n">
+      <c r="K74" s="9" t="n">
         <v>46184614134536</v>
       </c>
       <c r="L74" s="2" t="s">
@@ -5863,7 +5869,7 @@
       <c r="J75" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="K75" s="0" t="n">
+      <c r="K75" s="9" t="n">
         <v>12905351749025</v>
       </c>
       <c r="L75" s="2" t="s">
@@ -5919,7 +5925,7 @@
       <c r="J76" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="K76" s="0" t="n">
+      <c r="K76" s="9" t="n">
         <v>68752538027307</v>
       </c>
       <c r="L76" s="2" t="s">
@@ -5975,7 +5981,7 @@
       <c r="J77" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="K77" s="0" t="n">
+      <c r="K77" s="9" t="n">
         <v>98720908153351</v>
       </c>
       <c r="L77" s="2" t="s">
@@ -6031,7 +6037,7 @@
       <c r="J78" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K78" s="0" t="n">
+      <c r="K78" s="9" t="n">
         <v>55348001664418</v>
       </c>
       <c r="L78" s="2" t="s">
@@ -6087,7 +6093,7 @@
       <c r="J79" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K79" s="0" t="n">
+      <c r="K79" s="9" t="n">
         <v>30774456710067</v>
       </c>
       <c r="L79" s="2" t="s">
@@ -6143,7 +6149,7 @@
       <c r="J80" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="K80" s="0" t="n">
+      <c r="K80" s="9" t="n">
         <v>68564923891739</v>
       </c>
       <c r="L80" s="2" t="s">
@@ -6199,7 +6205,7 @@
       <c r="J81" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="K81" s="0" t="n">
+      <c r="K81" s="9" t="n">
         <v>50345433926955</v>
       </c>
       <c r="L81" s="2" t="s">
@@ -6255,7 +6261,7 @@
       <c r="J82" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="K82" s="0" t="n">
+      <c r="K82" s="9" t="n">
         <v>31052178275457</v>
       </c>
       <c r="L82" s="2" t="s">
@@ -6311,7 +6317,7 @@
       <c r="J83" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K83" s="0" t="n">
+      <c r="K83" s="9" t="n">
         <v>85762223738771</v>
       </c>
       <c r="L83" s="2" t="s">
@@ -6367,7 +6373,7 @@
       <c r="J84" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="K84" s="0" t="n">
+      <c r="K84" s="9" t="n">
         <v>70198266636742</v>
       </c>
       <c r="L84" s="2" t="s">
@@ -6423,7 +6429,7 @@
       <c r="J85" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="K85" s="0" t="n">
+      <c r="K85" s="9" t="n">
         <v>97640415842146</v>
       </c>
       <c r="L85" s="2" t="s">
@@ -6479,7 +6485,7 @@
       <c r="J86" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="K86" s="0" t="n">
+      <c r="K86" s="9" t="n">
         <v>34822992533965</v>
       </c>
       <c r="L86" s="2" t="s">
@@ -6535,7 +6541,7 @@
       <c r="J87" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="K87" s="0" t="n">
+      <c r="K87" s="9" t="n">
         <v>21999041322458</v>
       </c>
       <c r="L87" s="2" t="s">
@@ -6591,7 +6597,7 @@
       <c r="J88" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K88" s="0" t="n">
+      <c r="K88" s="9" t="n">
         <v>28480740716832</v>
       </c>
       <c r="L88" s="2" t="s">
@@ -6647,7 +6653,7 @@
       <c r="J89" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="K89" s="0" t="n">
+      <c r="K89" s="9" t="n">
         <v>12007701187044</v>
       </c>
       <c r="L89" s="2" t="s">
@@ -6703,7 +6709,7 @@
       <c r="J90" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="K90" s="0" t="n">
+      <c r="K90" s="9" t="n">
         <v>52542745485413</v>
       </c>
       <c r="L90" s="2" t="s">
@@ -6759,7 +6765,7 @@
       <c r="J91" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="K91" s="0" t="n">
+      <c r="K91" s="9" t="n">
         <v>55213723441930</v>
       </c>
       <c r="L91" s="2" t="s">
@@ -6815,7 +6821,7 @@
       <c r="J92" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="K92" s="0" t="n">
+      <c r="K92" s="9" t="n">
         <v>47989557632928</v>
       </c>
       <c r="L92" s="2" t="s">
@@ -6871,7 +6877,7 @@
       <c r="J93" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="K93" s="0" t="n">
+      <c r="K93" s="9" t="n">
         <v>34077609518227</v>
       </c>
       <c r="L93" s="2" t="s">
@@ -6927,7 +6933,7 @@
       <c r="J94" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="K94" s="0" t="n">
+      <c r="K94" s="9" t="n">
         <v>94149840457049</v>
       </c>
       <c r="L94" s="2" t="s">
@@ -6983,7 +6989,7 @@
       <c r="J95" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="K95" s="0" t="n">
+      <c r="K95" s="9" t="n">
         <v>49726664353560</v>
       </c>
       <c r="L95" s="2" t="s">
@@ -7039,7 +7045,7 @@
       <c r="J96" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="K96" s="0" t="n">
+      <c r="K96" s="9" t="n">
         <v>51107856020180</v>
       </c>
       <c r="L96" s="2" t="s">
@@ -7095,7 +7101,7 @@
       <c r="J97" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="K97" s="0" t="n">
+      <c r="K97" s="9" t="n">
         <v>18147609107602</v>
       </c>
       <c r="L97" s="2" t="s">
@@ -7151,7 +7157,7 @@
       <c r="J98" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="K98" s="0" t="n">
+      <c r="K98" s="9" t="n">
         <v>58270370800401</v>
       </c>
       <c r="L98" s="2" t="s">
@@ -7207,7 +7213,7 @@
       <c r="J99" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="K99" s="0" t="n">
+      <c r="K99" s="9" t="n">
         <v>25903365253926</v>
       </c>
       <c r="L99" s="2" t="s">
@@ -7263,7 +7269,7 @@
       <c r="J100" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="K100" s="0" t="n">
+      <c r="K100" s="9" t="n">
         <v>81093655936224</v>
       </c>
       <c r="L100" s="2" t="s">
@@ -7319,7 +7325,7 @@
       <c r="J101" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="K101" s="0" t="n">
+      <c r="K101" s="9" t="n">
         <v>64299921779656</v>
       </c>
       <c r="L101" s="2" t="s">
@@ -7375,7 +7381,7 @@
       <c r="J102" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="K102" s="0" t="n">
+      <c r="K102" s="9" t="n">
         <v>67414121775440</v>
       </c>
       <c r="L102" s="2" t="s">
@@ -7431,7 +7437,7 @@
       <c r="J103" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="K103" s="0" t="n">
+      <c r="K103" s="9" t="n">
         <v>43691172281110</v>
       </c>
       <c r="L103" s="2" t="s">
@@ -7487,7 +7493,7 @@
       <c r="J104" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="K104" s="0" t="n">
+      <c r="K104" s="9" t="n">
         <v>82184561311841</v>
       </c>
       <c r="L104" s="2" t="s">
@@ -7543,7 +7549,7 @@
       <c r="J105" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="K105" s="0" t="n">
+      <c r="K105" s="9" t="n">
         <v>11634228763467</v>
       </c>
       <c r="L105" s="2" t="s">
@@ -7599,7 +7605,7 @@
       <c r="J106" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="K106" s="0" t="n">
+      <c r="K106" s="9" t="n">
         <v>54061783574524</v>
       </c>
       <c r="L106" s="2" t="s">
@@ -7655,7 +7661,7 @@
       <c r="J107" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="K107" s="0" t="n">
+      <c r="K107" s="9" t="n">
         <v>49243897834070</v>
       </c>
       <c r="L107" s="2" t="s">
@@ -7721,19 +7727,19 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>480</v>
       </c>
       <c r="F2" s="7" t="s">

</xml_diff>

<commit_message>
remove GTIN because of improper format
</commit_message>
<xml_diff>
--- a/normalized-data/square-mass-import-catalog_usa.xlsx
+++ b/normalized-data/square-mass-import-catalog_usa.xlsx
@@ -1715,10 +1715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AF107"/>
+  <dimension ref="A2:AF119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L105" activeCellId="0" sqref="L105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7:K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1734,7 +1734,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="186.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="62.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="37.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="37.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="94.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="51.22"/>
@@ -2049,9 +2049,7 @@
       <c r="J7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="9" t="n">
-        <v>14109604604858</v>
-      </c>
+      <c r="K7" s="9"/>
       <c r="L7" s="2" t="s">
         <v>61</v>
       </c>
@@ -2117,9 +2115,7 @@
       <c r="J8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="9" t="n">
-        <v>14202221654343</v>
-      </c>
+      <c r="K8" s="9"/>
       <c r="L8" s="2" t="s">
         <v>61</v>
       </c>
@@ -2173,9 +2169,7 @@
       <c r="J9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="9" t="n">
-        <v>10289338790688</v>
-      </c>
+      <c r="K9" s="9"/>
       <c r="L9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2229,9 +2223,7 @@
       <c r="J10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="9" t="n">
-        <v>40290832470549</v>
-      </c>
+      <c r="K10" s="9"/>
       <c r="L10" s="2" t="s">
         <v>61</v>
       </c>
@@ -2285,9 +2277,7 @@
       <c r="J11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="9" t="n">
-        <v>84207900225560</v>
-      </c>
+      <c r="K11" s="9"/>
       <c r="L11" s="2" t="s">
         <v>61</v>
       </c>
@@ -2341,9 +2331,7 @@
       <c r="J12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="9" t="n">
-        <v>14722003109376</v>
-      </c>
+      <c r="K12" s="9"/>
       <c r="L12" s="2" t="s">
         <v>61</v>
       </c>
@@ -2397,9 +2385,7 @@
       <c r="J13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="9" t="n">
-        <v>73777516987868</v>
-      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="2" t="s">
         <v>61</v>
       </c>
@@ -2453,9 +2439,7 @@
       <c r="J14" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="9" t="n">
-        <v>51162143363027</v>
-      </c>
+      <c r="K14" s="9"/>
       <c r="L14" s="2" t="s">
         <v>61</v>
       </c>
@@ -2509,9 +2493,7 @@
       <c r="J15" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="9" t="n">
-        <v>99305262963586</v>
-      </c>
+      <c r="K15" s="9"/>
       <c r="L15" s="2" t="s">
         <v>61</v>
       </c>
@@ -2565,9 +2547,7 @@
       <c r="J16" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="K16" s="9" t="n">
-        <v>42132902332521</v>
-      </c>
+      <c r="K16" s="9"/>
       <c r="L16" s="2" t="s">
         <v>61</v>
       </c>
@@ -2621,9 +2601,7 @@
       <c r="J17" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="K17" s="9" t="n">
-        <v>49257718277257</v>
-      </c>
+      <c r="K17" s="9"/>
       <c r="L17" s="2" t="s">
         <v>61</v>
       </c>
@@ -2677,9 +2655,7 @@
       <c r="J18" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="9" t="n">
-        <v>23580959145415</v>
-      </c>
+      <c r="K18" s="9"/>
       <c r="L18" s="2" t="s">
         <v>61</v>
       </c>
@@ -2733,9 +2709,7 @@
       <c r="J19" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="K19" s="9" t="n">
-        <v>69125978120871</v>
-      </c>
+      <c r="K19" s="9"/>
       <c r="L19" s="2" t="s">
         <v>61</v>
       </c>
@@ -2789,9 +2763,7 @@
       <c r="J20" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K20" s="9" t="n">
-        <v>65859647272720</v>
-      </c>
+      <c r="K20" s="9"/>
       <c r="L20" s="2" t="s">
         <v>61</v>
       </c>
@@ -2845,9 +2817,7 @@
       <c r="J21" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="K21" s="9" t="n">
-        <v>80157313608196</v>
-      </c>
+      <c r="K21" s="9"/>
       <c r="L21" s="2" t="s">
         <v>61</v>
       </c>
@@ -2901,9 +2871,7 @@
       <c r="J22" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="K22" s="9" t="n">
-        <v>58468893137835</v>
-      </c>
+      <c r="K22" s="9"/>
       <c r="L22" s="2" t="s">
         <v>61</v>
       </c>
@@ -2957,9 +2925,7 @@
       <c r="J23" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="9" t="n">
-        <v>24655840280891</v>
-      </c>
+      <c r="K23" s="9"/>
       <c r="L23" s="2" t="s">
         <v>61</v>
       </c>
@@ -3013,9 +2979,7 @@
       <c r="J24" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="K24" s="9" t="n">
-        <v>93490705034401</v>
-      </c>
+      <c r="K24" s="9"/>
       <c r="L24" s="2" t="s">
         <v>61</v>
       </c>
@@ -3069,9 +3033,7 @@
       <c r="J25" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="K25" s="9" t="n">
-        <v>73105115630711</v>
-      </c>
+      <c r="K25" s="9"/>
       <c r="L25" s="2" t="s">
         <v>61</v>
       </c>
@@ -3125,9 +3087,7 @@
       <c r="J26" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K26" s="9" t="n">
-        <v>86685277622874</v>
-      </c>
+      <c r="K26" s="9"/>
       <c r="L26" s="2" t="s">
         <v>61</v>
       </c>
@@ -3181,9 +3141,7 @@
       <c r="J27" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K27" s="9" t="n">
-        <v>23761784959629</v>
-      </c>
+      <c r="K27" s="9"/>
       <c r="L27" s="2" t="s">
         <v>61</v>
       </c>
@@ -3237,9 +3195,7 @@
       <c r="J28" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="K28" s="9" t="n">
-        <v>51080830461219</v>
-      </c>
+      <c r="K28" s="9"/>
       <c r="L28" s="2" t="s">
         <v>61</v>
       </c>
@@ -3293,9 +3249,7 @@
       <c r="J29" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="K29" s="9" t="n">
-        <v>41418400223058</v>
-      </c>
+      <c r="K29" s="9"/>
       <c r="L29" s="2" t="s">
         <v>61</v>
       </c>
@@ -3349,9 +3303,7 @@
       <c r="J30" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K30" s="9" t="n">
-        <v>93758042485807</v>
-      </c>
+      <c r="K30" s="9"/>
       <c r="L30" s="2" t="s">
         <v>61</v>
       </c>
@@ -3405,9 +3357,7 @@
       <c r="J31" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K31" s="9" t="n">
-        <v>52171972512477</v>
-      </c>
+      <c r="K31" s="9"/>
       <c r="L31" s="2" t="s">
         <v>61</v>
       </c>
@@ -3461,9 +3411,7 @@
       <c r="J32" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K32" s="9" t="n">
-        <v>21583519874323</v>
-      </c>
+      <c r="K32" s="9"/>
       <c r="L32" s="2" t="s">
         <v>61</v>
       </c>
@@ -3517,9 +3465,7 @@
       <c r="J33" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="K33" s="9" t="n">
-        <v>26736626793030</v>
-      </c>
+      <c r="K33" s="9"/>
       <c r="L33" s="2" t="s">
         <v>61</v>
       </c>
@@ -3573,9 +3519,7 @@
       <c r="J34" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K34" s="9" t="n">
-        <v>12284011325362</v>
-      </c>
+      <c r="K34" s="9"/>
       <c r="L34" s="2" t="s">
         <v>61</v>
       </c>
@@ -3629,9 +3573,7 @@
       <c r="J35" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="K35" s="9" t="n">
-        <v>53666117476789</v>
-      </c>
+      <c r="K35" s="9"/>
       <c r="L35" s="2" t="s">
         <v>61</v>
       </c>
@@ -3685,9 +3627,7 @@
       <c r="J36" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="K36" s="9" t="n">
-        <v>75970202836561</v>
-      </c>
+      <c r="K36" s="9"/>
       <c r="L36" s="2" t="s">
         <v>61</v>
       </c>
@@ -3741,9 +3681,7 @@
       <c r="J37" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="K37" s="9" t="n">
-        <v>61327144407778</v>
-      </c>
+      <c r="K37" s="9"/>
       <c r="L37" s="2" t="s">
         <v>61</v>
       </c>
@@ -3797,9 +3735,7 @@
       <c r="J38" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="K38" s="9" t="n">
-        <v>45788508647136</v>
-      </c>
+      <c r="K38" s="9"/>
       <c r="L38" s="2" t="s">
         <v>61</v>
       </c>
@@ -3853,9 +3789,7 @@
       <c r="J39" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="K39" s="9" t="n">
-        <v>20127249361160</v>
-      </c>
+      <c r="K39" s="9"/>
       <c r="L39" s="2" t="s">
         <v>61</v>
       </c>
@@ -3909,9 +3843,7 @@
       <c r="J40" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="K40" s="9" t="n">
-        <v>62190360827574</v>
-      </c>
+      <c r="K40" s="9"/>
       <c r="L40" s="2" t="s">
         <v>61</v>
       </c>
@@ -3965,9 +3897,7 @@
       <c r="J41" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="K41" s="9" t="n">
-        <v>19459747163476</v>
-      </c>
+      <c r="K41" s="9"/>
       <c r="L41" s="2" t="s">
         <v>61</v>
       </c>
@@ -4021,9 +3951,7 @@
       <c r="J42" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="K42" s="9" t="n">
-        <v>46746380394391</v>
-      </c>
+      <c r="K42" s="9"/>
       <c r="L42" s="2" t="s">
         <v>61</v>
       </c>
@@ -4077,9 +4005,7 @@
       <c r="J43" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="K43" s="9" t="n">
-        <v>20256258825006</v>
-      </c>
+      <c r="K43" s="9"/>
       <c r="L43" s="2" t="s">
         <v>61</v>
       </c>
@@ -4133,9 +4059,7 @@
       <c r="J44" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="K44" s="9" t="n">
-        <v>71473469057315</v>
-      </c>
+      <c r="K44" s="9"/>
       <c r="L44" s="2" t="s">
         <v>61</v>
       </c>
@@ -4189,9 +4113,7 @@
       <c r="J45" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="K45" s="9" t="n">
-        <v>35224346795683</v>
-      </c>
+      <c r="K45" s="9"/>
       <c r="L45" s="2" t="s">
         <v>61</v>
       </c>
@@ -4245,9 +4167,7 @@
       <c r="J46" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="K46" s="9" t="n">
-        <v>45734082687422</v>
-      </c>
+      <c r="K46" s="9"/>
       <c r="L46" s="2" t="s">
         <v>61</v>
       </c>
@@ -4301,9 +4221,7 @@
       <c r="J47" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="K47" s="9" t="n">
-        <v>25090603661905</v>
-      </c>
+      <c r="K47" s="9"/>
       <c r="L47" s="2" t="s">
         <v>61</v>
       </c>
@@ -4357,9 +4275,7 @@
       <c r="J48" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="K48" s="9" t="n">
-        <v>84952970015668</v>
-      </c>
+      <c r="K48" s="9"/>
       <c r="L48" s="2" t="s">
         <v>61</v>
       </c>
@@ -4413,9 +4329,7 @@
       <c r="J49" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="K49" s="9" t="n">
-        <v>76416879474381</v>
-      </c>
+      <c r="K49" s="9"/>
       <c r="L49" s="2" t="s">
         <v>61</v>
       </c>
@@ -4469,9 +4383,7 @@
       <c r="J50" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="K50" s="9" t="n">
-        <v>16269018549201</v>
-      </c>
+      <c r="K50" s="9"/>
       <c r="L50" s="2" t="s">
         <v>61</v>
       </c>
@@ -4525,9 +4437,7 @@
       <c r="J51" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="K51" s="9" t="n">
-        <v>36007938913287</v>
-      </c>
+      <c r="K51" s="9"/>
       <c r="L51" s="2" t="s">
         <v>61</v>
       </c>
@@ -4581,9 +4491,7 @@
       <c r="J52" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="K52" s="9" t="n">
-        <v>24525747669281</v>
-      </c>
+      <c r="K52" s="9"/>
       <c r="L52" s="2" t="s">
         <v>61</v>
       </c>
@@ -4637,9 +4545,7 @@
       <c r="J53" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="K53" s="9" t="n">
-        <v>26196313329786</v>
-      </c>
+      <c r="K53" s="9"/>
       <c r="L53" s="2" t="s">
         <v>61</v>
       </c>
@@ -4693,9 +4599,7 @@
       <c r="J54" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="K54" s="9" t="n">
-        <v>20862838477345</v>
-      </c>
+      <c r="K54" s="9"/>
       <c r="L54" s="2" t="s">
         <v>61</v>
       </c>
@@ -4749,9 +4653,7 @@
       <c r="J55" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="K55" s="9" t="n">
-        <v>36037284563664</v>
-      </c>
+      <c r="K55" s="9"/>
       <c r="L55" s="2" t="s">
         <v>61</v>
       </c>
@@ -4805,9 +4707,7 @@
       <c r="J56" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="K56" s="9" t="n">
-        <v>13193681859339</v>
-      </c>
+      <c r="K56" s="9"/>
       <c r="L56" s="2" t="s">
         <v>61</v>
       </c>
@@ -4861,9 +4761,7 @@
       <c r="J57" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="K57" s="9" t="n">
-        <v>86763178062714</v>
-      </c>
+      <c r="K57" s="9"/>
       <c r="L57" s="2" t="s">
         <v>61</v>
       </c>
@@ -4917,9 +4815,7 @@
       <c r="J58" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="K58" s="9" t="n">
-        <v>20530814931315</v>
-      </c>
+      <c r="K58" s="9"/>
       <c r="L58" s="2" t="s">
         <v>61</v>
       </c>
@@ -4973,9 +4869,7 @@
       <c r="J59" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="K59" s="9" t="n">
-        <v>63318658338474</v>
-      </c>
+      <c r="K59" s="9"/>
       <c r="L59" s="2" t="s">
         <v>61</v>
       </c>
@@ -5029,9 +4923,7 @@
       <c r="J60" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="K60" s="9" t="n">
-        <v>16310871290403</v>
-      </c>
+      <c r="K60" s="9"/>
       <c r="L60" s="2" t="s">
         <v>61</v>
       </c>
@@ -5085,9 +4977,7 @@
       <c r="J61" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="K61" s="9" t="n">
-        <v>65940494145215</v>
-      </c>
+      <c r="K61" s="9"/>
       <c r="L61" s="2" t="s">
         <v>61</v>
       </c>
@@ -5141,9 +5031,7 @@
       <c r="J62" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="K62" s="9" t="n">
-        <v>22515530946973</v>
-      </c>
+      <c r="K62" s="9"/>
       <c r="L62" s="2" t="s">
         <v>61</v>
       </c>
@@ -5197,9 +5085,7 @@
       <c r="J63" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="K63" s="9" t="n">
-        <v>76547149292154</v>
-      </c>
+      <c r="K63" s="9"/>
       <c r="L63" s="2" t="s">
         <v>61</v>
       </c>
@@ -5253,9 +5139,7 @@
       <c r="J64" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="K64" s="9" t="n">
-        <v>92842924373813</v>
-      </c>
+      <c r="K64" s="9"/>
       <c r="L64" s="2" t="s">
         <v>61</v>
       </c>
@@ -5309,9 +5193,7 @@
       <c r="J65" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="K65" s="9" t="n">
-        <v>73064086186736</v>
-      </c>
+      <c r="K65" s="9"/>
       <c r="L65" s="2" t="s">
         <v>61</v>
       </c>
@@ -5365,9 +5247,7 @@
       <c r="J66" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="K66" s="9" t="n">
-        <v>13567700390896</v>
-      </c>
+      <c r="K66" s="9"/>
       <c r="L66" s="2" t="s">
         <v>61</v>
       </c>
@@ -5421,9 +5301,7 @@
       <c r="J67" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="K67" s="9" t="n">
-        <v>52280020167217</v>
-      </c>
+      <c r="K67" s="9"/>
       <c r="L67" s="2" t="s">
         <v>61</v>
       </c>
@@ -5477,9 +5355,7 @@
       <c r="J68" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K68" s="9" t="n">
-        <v>55225619530351</v>
-      </c>
+      <c r="K68" s="9"/>
       <c r="L68" s="2" t="s">
         <v>61</v>
       </c>
@@ -5533,9 +5409,7 @@
       <c r="J69" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="K69" s="9" t="n">
-        <v>66882207361884</v>
-      </c>
+      <c r="K69" s="9"/>
       <c r="L69" s="2" t="s">
         <v>61</v>
       </c>
@@ -5589,9 +5463,7 @@
       <c r="J70" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="K70" s="9" t="n">
-        <v>19263536217596</v>
-      </c>
+      <c r="K70" s="9"/>
       <c r="L70" s="2" t="s">
         <v>61</v>
       </c>
@@ -5645,9 +5517,7 @@
       <c r="J71" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="K71" s="9" t="n">
-        <v>88129625450959</v>
-      </c>
+      <c r="K71" s="9"/>
       <c r="L71" s="2" t="s">
         <v>61</v>
       </c>
@@ -5701,9 +5571,7 @@
       <c r="J72" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="K72" s="9" t="n">
-        <v>67801006981945</v>
-      </c>
+      <c r="K72" s="9"/>
       <c r="L72" s="2" t="s">
         <v>61</v>
       </c>
@@ -5757,9 +5625,7 @@
       <c r="J73" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="K73" s="9" t="n">
-        <v>62159138423123</v>
-      </c>
+      <c r="K73" s="9"/>
       <c r="L73" s="2" t="s">
         <v>61</v>
       </c>
@@ -5813,9 +5679,7 @@
       <c r="J74" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="K74" s="9" t="n">
-        <v>46184614134536</v>
-      </c>
+      <c r="K74" s="9"/>
       <c r="L74" s="2" t="s">
         <v>61</v>
       </c>
@@ -5869,9 +5733,7 @@
       <c r="J75" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="K75" s="9" t="n">
-        <v>12905351749025</v>
-      </c>
+      <c r="K75" s="9"/>
       <c r="L75" s="2" t="s">
         <v>61</v>
       </c>
@@ -5925,9 +5787,7 @@
       <c r="J76" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="K76" s="9" t="n">
-        <v>68752538027307</v>
-      </c>
+      <c r="K76" s="9"/>
       <c r="L76" s="2" t="s">
         <v>61</v>
       </c>
@@ -5981,9 +5841,7 @@
       <c r="J77" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="K77" s="9" t="n">
-        <v>98720908153351</v>
-      </c>
+      <c r="K77" s="9"/>
       <c r="L77" s="2" t="s">
         <v>61</v>
       </c>
@@ -6037,9 +5895,7 @@
       <c r="J78" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="K78" s="9" t="n">
-        <v>55348001664418</v>
-      </c>
+      <c r="K78" s="9"/>
       <c r="L78" s="2" t="s">
         <v>61</v>
       </c>
@@ -6093,9 +5949,7 @@
       <c r="J79" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K79" s="9" t="n">
-        <v>30774456710067</v>
-      </c>
+      <c r="K79" s="9"/>
       <c r="L79" s="2" t="s">
         <v>61</v>
       </c>
@@ -6149,9 +6003,7 @@
       <c r="J80" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="K80" s="9" t="n">
-        <v>68564923891739</v>
-      </c>
+      <c r="K80" s="9"/>
       <c r="L80" s="2" t="s">
         <v>61</v>
       </c>
@@ -6205,9 +6057,7 @@
       <c r="J81" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="K81" s="9" t="n">
-        <v>50345433926955</v>
-      </c>
+      <c r="K81" s="9"/>
       <c r="L81" s="2" t="s">
         <v>61</v>
       </c>
@@ -6261,9 +6111,7 @@
       <c r="J82" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="K82" s="9" t="n">
-        <v>31052178275457</v>
-      </c>
+      <c r="K82" s="9"/>
       <c r="L82" s="2" t="s">
         <v>61</v>
       </c>
@@ -6317,9 +6165,7 @@
       <c r="J83" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K83" s="9" t="n">
-        <v>85762223738771</v>
-      </c>
+      <c r="K83" s="9"/>
       <c r="L83" s="2" t="s">
         <v>61</v>
       </c>
@@ -6373,9 +6219,7 @@
       <c r="J84" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="K84" s="9" t="n">
-        <v>70198266636742</v>
-      </c>
+      <c r="K84" s="9"/>
       <c r="L84" s="2" t="s">
         <v>61</v>
       </c>
@@ -6429,9 +6273,7 @@
       <c r="J85" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="K85" s="9" t="n">
-        <v>97640415842146</v>
-      </c>
+      <c r="K85" s="9"/>
       <c r="L85" s="2" t="s">
         <v>61</v>
       </c>
@@ -6485,9 +6327,7 @@
       <c r="J86" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="K86" s="9" t="n">
-        <v>34822992533965</v>
-      </c>
+      <c r="K86" s="9"/>
       <c r="L86" s="2" t="s">
         <v>61</v>
       </c>
@@ -6541,9 +6381,7 @@
       <c r="J87" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="K87" s="9" t="n">
-        <v>21999041322458</v>
-      </c>
+      <c r="K87" s="9"/>
       <c r="L87" s="2" t="s">
         <v>61</v>
       </c>
@@ -6597,9 +6435,7 @@
       <c r="J88" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K88" s="9" t="n">
-        <v>28480740716832</v>
-      </c>
+      <c r="K88" s="9"/>
       <c r="L88" s="2" t="s">
         <v>61</v>
       </c>
@@ -6653,9 +6489,7 @@
       <c r="J89" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="K89" s="9" t="n">
-        <v>12007701187044</v>
-      </c>
+      <c r="K89" s="9"/>
       <c r="L89" s="2" t="s">
         <v>61</v>
       </c>
@@ -6709,9 +6543,7 @@
       <c r="J90" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="K90" s="9" t="n">
-        <v>52542745485413</v>
-      </c>
+      <c r="K90" s="9"/>
       <c r="L90" s="2" t="s">
         <v>61</v>
       </c>
@@ -6765,9 +6597,7 @@
       <c r="J91" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="K91" s="9" t="n">
-        <v>55213723441930</v>
-      </c>
+      <c r="K91" s="9"/>
       <c r="L91" s="2" t="s">
         <v>61</v>
       </c>
@@ -6821,9 +6651,7 @@
       <c r="J92" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="K92" s="9" t="n">
-        <v>47989557632928</v>
-      </c>
+      <c r="K92" s="9"/>
       <c r="L92" s="2" t="s">
         <v>61</v>
       </c>
@@ -6877,9 +6705,7 @@
       <c r="J93" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="K93" s="9" t="n">
-        <v>34077609518227</v>
-      </c>
+      <c r="K93" s="9"/>
       <c r="L93" s="2" t="s">
         <v>61</v>
       </c>
@@ -6933,9 +6759,7 @@
       <c r="J94" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="K94" s="9" t="n">
-        <v>94149840457049</v>
-      </c>
+      <c r="K94" s="9"/>
       <c r="L94" s="2" t="s">
         <v>61</v>
       </c>
@@ -6989,9 +6813,7 @@
       <c r="J95" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="K95" s="9" t="n">
-        <v>49726664353560</v>
-      </c>
+      <c r="K95" s="9"/>
       <c r="L95" s="2" t="s">
         <v>61</v>
       </c>
@@ -7045,9 +6867,7 @@
       <c r="J96" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="K96" s="9" t="n">
-        <v>51107856020180</v>
-      </c>
+      <c r="K96" s="9"/>
       <c r="L96" s="2" t="s">
         <v>61</v>
       </c>
@@ -7101,9 +6921,7 @@
       <c r="J97" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="K97" s="9" t="n">
-        <v>18147609107602</v>
-      </c>
+      <c r="K97" s="9"/>
       <c r="L97" s="2" t="s">
         <v>61</v>
       </c>
@@ -7157,9 +6975,7 @@
       <c r="J98" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="K98" s="9" t="n">
-        <v>58270370800401</v>
-      </c>
+      <c r="K98" s="9"/>
       <c r="L98" s="2" t="s">
         <v>61</v>
       </c>
@@ -7213,9 +7029,7 @@
       <c r="J99" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="K99" s="9" t="n">
-        <v>25903365253926</v>
-      </c>
+      <c r="K99" s="9"/>
       <c r="L99" s="2" t="s">
         <v>61</v>
       </c>
@@ -7269,9 +7083,7 @@
       <c r="J100" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="K100" s="9" t="n">
-        <v>81093655936224</v>
-      </c>
+      <c r="K100" s="9"/>
       <c r="L100" s="2" t="s">
         <v>61</v>
       </c>
@@ -7325,9 +7137,7 @@
       <c r="J101" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="K101" s="9" t="n">
-        <v>64299921779656</v>
-      </c>
+      <c r="K101" s="9"/>
       <c r="L101" s="2" t="s">
         <v>61</v>
       </c>
@@ -7381,9 +7191,7 @@
       <c r="J102" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="K102" s="9" t="n">
-        <v>67414121775440</v>
-      </c>
+      <c r="K102" s="9"/>
       <c r="L102" s="2" t="s">
         <v>61</v>
       </c>
@@ -7437,9 +7245,7 @@
       <c r="J103" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="K103" s="9" t="n">
-        <v>43691172281110</v>
-      </c>
+      <c r="K103" s="9"/>
       <c r="L103" s="2" t="s">
         <v>61</v>
       </c>
@@ -7493,9 +7299,7 @@
       <c r="J104" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="K104" s="9" t="n">
-        <v>82184561311841</v>
-      </c>
+      <c r="K104" s="9"/>
       <c r="L104" s="2" t="s">
         <v>61</v>
       </c>
@@ -7549,9 +7353,7 @@
       <c r="J105" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="K105" s="9" t="n">
-        <v>11634228763467</v>
-      </c>
+      <c r="K105" s="9"/>
       <c r="L105" s="2" t="s">
         <v>61</v>
       </c>
@@ -7605,9 +7407,7 @@
       <c r="J106" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="K106" s="9" t="n">
-        <v>54061783574524</v>
-      </c>
+      <c r="K106" s="9"/>
       <c r="L106" s="2" t="s">
         <v>61</v>
       </c>
@@ -7661,9 +7461,7 @@
       <c r="J107" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="K107" s="9" t="n">
-        <v>49243897834070</v>
-      </c>
+      <c r="K107" s="9"/>
       <c r="L107" s="2" t="s">
         <v>61</v>
       </c>
@@ -7695,6 +7493,18 @@
         <v>64</v>
       </c>
     </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
@@ -7718,7 +7528,7 @@
   <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K7:K119 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>